<commit_message>
adding module 7 discussion post code
adding module 7 discussion post code
</commit_message>
<xml_diff>
--- a/Integer Programming and Nonlinear Programming/Assignment 3 Supporting Workbook.xlsx
+++ b/Integer Programming and Nonlinear Programming/Assignment 3 Supporting Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2df8f4c56c849a7f/Desktop/Github/Decision-Analytics/Integer Programming and Nonlinear Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14227" documentId="8_{7A0BABFD-A69F-482A-B851-72D547AF9D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6202716-149D-43F2-B9F6-CC25959E9B6F}"/>
+  <xr:revisionPtr revIDLastSave="14232" documentId="8_{7A0BABFD-A69F-482A-B851-72D547AF9D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{925AFADE-7AE6-4DA3-BE0F-4A08D8F214AD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="600" yWindow="264" windowWidth="13152" windowHeight="11976" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Question 1B" sheetId="6" r:id="rId1"/>
@@ -901,7 +901,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -915,32 +915,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -984,16 +960,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1014,9 +981,6 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1024,16 +988,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1050,52 +1011,94 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="0" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1415,148 +1418,148 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.7109375" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="29"/>
-    <col min="5" max="5" width="12.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="29"/>
+    <col min="3" max="4" width="9.140625" style="21"/>
+    <col min="5" max="5" width="12.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="56" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="33"/>
+      <c r="D2" s="60"/>
     </row>
     <row r="3" spans="1:7" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="5"/>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="24" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="38">
+      <c r="A4" s="58"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="27">
         <v>3.1578947368421053</v>
       </c>
-      <c r="D4" s="39">
+      <c r="D4" s="28">
         <v>2.9473684210526319</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="10.8" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="22">
         <v>4</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="22">
         <v>2</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="11">
         <v>-0.5</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="11">
         <v>-0.25</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="26">
         <f>(C6*C4)+(D6*D4)+(C7*(C4^2)) + (D7*(D4^2))</f>
         <v>11.368421052631579</v>
       </c>
-      <c r="F7" s="31"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:7" ht="10.8" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:7" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="63" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="12">
         <v>8000</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="12">
         <v>5000</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="13">
         <f>SUMPRODUCT($C$4:$D$4,C9:D9)</f>
         <v>40000</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="15">
         <v>40000</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="64"/>
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="16">
         <v>1</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="40">
+      <c r="D10" s="16"/>
+      <c r="E10" s="29">
         <f>SUMPRODUCT($C$4:$D$4,C10:D10)</f>
         <v>3.1578947368421053</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14" t="s">
+      <c r="A11" s="65"/>
+      <c r="B11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26">
+      <c r="C11" s="18"/>
+      <c r="D11" s="18">
         <v>1</v>
       </c>
-      <c r="E11" s="41">
+      <c r="E11" s="30">
         <f>SUMPRODUCT($C$4:$D$4,C11:D11)</f>
         <v>2.9473684210526319</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1577,36 +1580,36 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="29" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="29"/>
-    <col min="7" max="7" width="12.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="29"/>
+    <col min="3" max="3" width="14.140625" style="21" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" style="21"/>
+    <col min="7" max="7" width="12.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="56" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="60"/>
     </row>
     <row r="3" spans="1:9" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="5"/>
       <c r="C3" s="2" t="s">
         <v>15</v>
@@ -1622,28 +1625,28 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="43">
+      <c r="A4" s="58"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="31">
         <v>20.000602411219802</v>
       </c>
-      <c r="D4" s="43">
+      <c r="D4" s="31">
         <v>19.999332931320371</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="31">
         <v>20.000064359438539</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="31">
         <v>29.999999850989354</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
       <c r="F6"/>
@@ -1652,11 +1655,11 @@
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16" t="s">
+      <c r="A7" s="67"/>
+      <c r="B7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="44">
+      <c r="C7" s="32">
         <f>F4*(F4-C4)*(F4-D4)*(F4-E4)</f>
         <v>29999.999282154888</v>
       </c>
@@ -1666,15 +1669,15 @@
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
+      <c r="A8" s="62"/>
       <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="45">
+      <c r="C8" s="33">
         <f>IF(C7&gt;0,C7^0.5,"Invalid Value")</f>
         <v>173.20507868464736</v>
       </c>
-      <c r="D8" s="31"/>
+      <c r="D8" s="23"/>
       <c r="F8"/>
       <c r="G8"/>
       <c r="H8"/>
@@ -1682,224 +1685,224 @@
     </row>
     <row r="9" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="63" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="12">
         <v>1</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="12">
         <v>1</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="12">
         <v>1</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="12">
         <v>-2</v>
       </c>
-      <c r="G10" s="40">
+      <c r="G10" s="71">
         <f t="shared" ref="G10:G13" si="0">SUMPRODUCT($C$4:$F$4,C10:F10)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="64"/>
       <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="16">
         <v>1</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="16">
         <v>-1</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="16">
         <v>-1</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="40">
+      <c r="F11" s="16"/>
+      <c r="G11" s="71">
         <f t="shared" si="0"/>
         <v>-19.998794879539108</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="64"/>
       <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="16">
         <v>-1</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="16">
         <v>1</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="16">
         <v>-1</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="40">
+      <c r="F12" s="16"/>
+      <c r="G12" s="71">
         <f t="shared" si="0"/>
         <v>-20.00133383933797</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="16">
         <v>-1</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="16">
         <v>-1</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="16">
         <v>1</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="40">
+      <c r="F13" s="16"/>
+      <c r="G13" s="71">
         <f t="shared" si="0"/>
         <v>-19.99987098310163</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="64"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="16">
         <v>1</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="16">
         <v>1</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="16">
         <v>1</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="40">
+      <c r="F14" s="16"/>
+      <c r="G14" s="71">
         <f>SUMPRODUCT($C$4:$F$4,C14:F14)</f>
         <v>59.999999701978709</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="H14" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="17">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="16">
         <v>1</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="40">
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="71">
         <f>SUMPRODUCT($C$4:$F$4,C15:F15)</f>
         <v>20.000602411219802</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16">
         <v>1</v>
       </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="40">
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="71">
         <f>SUMPRODUCT($C$4:$F$4,C16:F16)</f>
         <v>19.999332931320371</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24">
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16">
         <v>1</v>
       </c>
-      <c r="F17" s="24"/>
-      <c r="G17" s="40">
+      <c r="F17" s="16"/>
+      <c r="G17" s="71">
         <f>SUMPRODUCT($C$4:$F$4,C17:F17)</f>
         <v>20.000064359438539</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14" t="s">
+      <c r="A18" s="65"/>
+      <c r="B18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26">
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18">
         <v>1</v>
       </c>
-      <c r="G18" s="41">
+      <c r="G18" s="72">
         <f>SUMPRODUCT($C$4:$F$4,C18:F18)</f>
         <v>29.999999850989354</v>
       </c>
-      <c r="H18" s="27" t="s">
+      <c r="H18" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1919,8 +1922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48A99513-077C-4A72-BCF8-2C00EDD18050}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -1928,11 +1931,11 @@
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="29" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="29"/>
+    <col min="4" max="4" width="14.140625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
@@ -1940,49 +1943,47 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="59" t="s">
+      <c r="A2" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="60"/>
-      <c r="F2" s="56"/>
+      <c r="E2" s="69"/>
     </row>
     <row r="3" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="58" t="s">
+      <c r="A3" s="57"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="61" t="s">
+      <c r="E3" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="56"/>
     </row>
     <row r="4" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="62">
+      <c r="A4" s="58"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="46">
         <v>47.070259167221572</v>
       </c>
-      <c r="E4" s="63">
+      <c r="E4" s="47">
         <v>4435.101700178373</v>
       </c>
-      <c r="F4" s="57"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E6"/>
@@ -1992,10 +1993,10 @@
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="64">
+      <c r="D7" s="48">
         <f>SUM(F10:F19)</f>
         <v>9249747.5583069511</v>
       </c>
@@ -2007,325 +2008,325 @@
     </row>
     <row r="8" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="63" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="54" t="s">
+      <c r="E9" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="54" t="s">
+      <c r="F9" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="54" t="s">
+      <c r="G9" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="54"/>
-      <c r="I9" s="55"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="42"/>
     </row>
     <row r="10" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="64"/>
       <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="51">
+      <c r="C10" s="38">
         <v>40</v>
       </c>
-      <c r="D10" s="65">
+      <c r="D10" s="49">
         <v>5958</v>
       </c>
-      <c r="E10" s="65">
+      <c r="E10" s="49">
         <f>($D$4*C10)+$E$4</f>
         <v>6317.9120668672358</v>
       </c>
-      <c r="F10" s="65">
+      <c r="F10" s="49">
         <f>(D10-E10)^2</f>
         <v>129536.69587664562</v>
       </c>
-      <c r="G10" s="66">
+      <c r="G10" s="50">
         <f>E10-($D$4*C10) - $E$4</f>
         <v>0</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="64"/>
       <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="51">
+      <c r="C11" s="38">
         <v>44</v>
       </c>
-      <c r="D11" s="65">
+      <c r="D11" s="49">
         <v>6662</v>
       </c>
-      <c r="E11" s="65">
+      <c r="E11" s="49">
         <f t="shared" ref="E11:E19" si="0">($D$4*C11)+$E$4</f>
         <v>6506.1931035361222</v>
       </c>
-      <c r="F11" s="65">
+      <c r="F11" s="49">
         <f t="shared" ref="F11:F19" si="1">(D11-E11)^2</f>
         <v>24275.788985705542</v>
       </c>
-      <c r="G11" s="66">
+      <c r="G11" s="50">
         <f t="shared" ref="G11:G19" si="2">E11-($D$4*C11) - $E$4</f>
         <v>0</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="64"/>
       <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="51">
+      <c r="C12" s="38">
         <v>48</v>
       </c>
-      <c r="D12" s="65">
+      <c r="D12" s="49">
         <v>6004</v>
       </c>
-      <c r="E12" s="65">
+      <c r="E12" s="49">
         <f t="shared" si="0"/>
         <v>6694.4741402050086</v>
       </c>
-      <c r="F12" s="65">
+      <c r="F12" s="49">
         <f t="shared" si="1"/>
         <v>476754.53829184582</v>
       </c>
-      <c r="G12" s="66">
+      <c r="G12" s="50">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="51">
+      <c r="C13" s="38">
         <v>48</v>
       </c>
-      <c r="D13" s="65">
+      <c r="D13" s="49">
         <v>6011</v>
       </c>
-      <c r="E13" s="65">
+      <c r="E13" s="49">
         <f t="shared" si="0"/>
         <v>6694.4741402050086</v>
       </c>
-      <c r="F13" s="65">
+      <c r="F13" s="49">
         <f t="shared" si="1"/>
         <v>467136.90032897569</v>
       </c>
-      <c r="G13" s="66">
+      <c r="G13" s="50">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="64"/>
       <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="51">
+      <c r="C14" s="38">
         <v>60</v>
       </c>
-      <c r="D14" s="65">
+      <c r="D14" s="49">
         <v>7250</v>
       </c>
-      <c r="E14" s="65">
+      <c r="E14" s="49">
         <f t="shared" si="0"/>
         <v>7259.3172502116668</v>
       </c>
-      <c r="F14" s="65">
+      <c r="F14" s="49">
         <f t="shared" si="1"/>
         <v>86.811151506804293</v>
       </c>
-      <c r="G14" s="66">
+      <c r="G14" s="50">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="H14" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="51">
+      <c r="C15" s="38">
         <v>70</v>
       </c>
-      <c r="D15" s="65">
+      <c r="D15" s="49">
         <v>8632</v>
       </c>
-      <c r="E15" s="65">
+      <c r="E15" s="49">
         <f t="shared" si="0"/>
         <v>7730.0198418838827</v>
       </c>
-      <c r="F15" s="65">
+      <c r="F15" s="49">
         <f t="shared" si="1"/>
         <v>813568.20563517592</v>
       </c>
-      <c r="G15" s="66">
+      <c r="G15" s="50">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="51">
+      <c r="C16" s="38">
         <v>72</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="49">
         <v>6964</v>
       </c>
-      <c r="E16" s="65">
+      <c r="E16" s="49">
         <f t="shared" si="0"/>
         <v>7824.1603602183259</v>
       </c>
-      <c r="F16" s="65">
+      <c r="F16" s="49">
         <f t="shared" si="1"/>
         <v>739875.84529092012</v>
       </c>
-      <c r="G16" s="66">
+      <c r="G16" s="50">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="51">
+      <c r="C17" s="38">
         <v>90</v>
       </c>
-      <c r="D17" s="65">
+      <c r="D17" s="49">
         <v>11097</v>
       </c>
-      <c r="E17" s="65">
+      <c r="E17" s="49">
         <f t="shared" si="0"/>
         <v>8671.4250252283146</v>
       </c>
-      <c r="F17" s="65">
+      <c r="F17" s="49">
         <f t="shared" si="1"/>
         <v>5883413.9582386622</v>
       </c>
-      <c r="G17" s="66">
+      <c r="G17" s="50">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
-      <c r="B18" s="47" t="s">
+      <c r="A18" s="70"/>
+      <c r="B18" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="51">
+      <c r="C18" s="38">
         <v>100</v>
       </c>
-      <c r="D18" s="65">
+      <c r="D18" s="49">
         <v>9107</v>
       </c>
-      <c r="E18" s="65">
+      <c r="E18" s="49">
         <f t="shared" si="0"/>
         <v>9142.1276169005305</v>
       </c>
-      <c r="F18" s="65">
+      <c r="F18" s="49">
         <f t="shared" si="1"/>
         <v>1233.9494691104348</v>
       </c>
-      <c r="G18" s="66">
+      <c r="G18" s="50">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="65"/>
+      <c r="B19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="52">
+      <c r="C19" s="39">
         <v>168</v>
       </c>
-      <c r="D19" s="67">
+      <c r="D19" s="51">
         <v>11498</v>
       </c>
-      <c r="E19" s="67">
+      <c r="E19" s="51">
         <f t="shared" si="0"/>
         <v>12342.905240271597</v>
       </c>
-      <c r="F19" s="67">
+      <c r="F19" s="51">
         <f t="shared" si="1"/>
         <v>713864.86503840506</v>
       </c>
-      <c r="G19" s="68">
+      <c r="G19" s="52">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H19" s="22" t="s">
+      <c r="H19" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="28">
+      <c r="I19" s="20">
         <v>0</v>
       </c>
     </row>
@@ -2345,7 +2346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9634EC-A93B-4362-AFB1-1E88630C0237}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -2354,11 +2355,11 @@
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="29"/>
+    <col min="4" max="4" width="15.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
@@ -2366,49 +2367,47 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="59" t="s">
+      <c r="A2" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="60"/>
-      <c r="F2" s="56"/>
+      <c r="E2" s="69"/>
     </row>
     <row r="3" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="58" t="s">
+      <c r="A3" s="57"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="61" t="s">
+      <c r="E3" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="56"/>
     </row>
     <row r="4" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="62">
+      <c r="A4" s="58"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="46">
         <v>153.67424630662782</v>
       </c>
-      <c r="E4" s="63">
+      <c r="E4" s="47">
         <v>-0.51243659019261856</v>
       </c>
-      <c r="F4" s="57"/>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E6"/>
@@ -2418,10 +2417,10 @@
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="64">
+      <c r="D7" s="48">
         <f>SUM(F10:F19)</f>
         <v>6834614.3499019416</v>
       </c>
@@ -2433,325 +2432,325 @@
     </row>
     <row r="8" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="63" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="54" t="s">
+      <c r="E9" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="54" t="s">
+      <c r="F9" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="69" t="s">
+      <c r="G9" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="54"/>
-      <c r="I9" s="55"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="42"/>
     </row>
     <row r="10" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="64"/>
       <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="51">
+      <c r="C10" s="38">
         <v>40</v>
       </c>
-      <c r="D10" s="65">
+      <c r="D10" s="49">
         <v>5958</v>
       </c>
-      <c r="E10" s="65">
+      <c r="E10" s="49">
         <f>($D$4*C10) + ($E$4*(C10^2))</f>
         <v>5327.0713079569232</v>
       </c>
-      <c r="F10" s="65">
+      <c r="F10" s="49">
         <f>(D10-E10)^2</f>
         <v>398071.01444318763</v>
       </c>
-      <c r="G10" s="70">
+      <c r="G10" s="54">
         <f>E10- ($D$4*C10) - ($E$4*C10^2)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="64"/>
       <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="51">
+      <c r="C11" s="38">
         <v>44</v>
       </c>
-      <c r="D11" s="65">
+      <c r="D11" s="49">
         <v>6662</v>
       </c>
-      <c r="E11" s="65">
+      <c r="E11" s="49">
         <f t="shared" ref="E11:E19" si="0">($D$4*C11) + ($E$4*(C11^2))</f>
         <v>5769.5895988787152</v>
       </c>
-      <c r="F11" s="65">
+      <c r="F11" s="49">
         <f t="shared" ref="F11:F19" si="1">(D11-E11)^2</f>
         <v>796396.32402945252</v>
       </c>
-      <c r="G11" s="70">
+      <c r="G11" s="54">
         <f t="shared" ref="G11:G19" si="2">E11- ($D$4*C11) - ($E$4*C11^2)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="64"/>
       <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="51">
+      <c r="C12" s="38">
         <v>48</v>
       </c>
-      <c r="D12" s="65">
+      <c r="D12" s="49">
         <v>6004</v>
       </c>
-      <c r="E12" s="65">
+      <c r="E12" s="49">
         <f t="shared" si="0"/>
         <v>6195.7099189143428</v>
       </c>
-      <c r="F12" s="65">
+      <c r="F12" s="49">
         <f t="shared" si="1"/>
         <v>36752.693010143885</v>
       </c>
-      <c r="G12" s="70">
+      <c r="G12" s="54">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="51">
+      <c r="C13" s="38">
         <v>48</v>
       </c>
-      <c r="D13" s="65">
+      <c r="D13" s="49">
         <v>6011</v>
       </c>
-      <c r="E13" s="65">
+      <c r="E13" s="49">
         <f t="shared" si="0"/>
         <v>6195.7099189143428</v>
       </c>
-      <c r="F13" s="65">
+      <c r="F13" s="49">
         <f t="shared" si="1"/>
         <v>34117.754145343082</v>
       </c>
-      <c r="G13" s="70">
+      <c r="G13" s="54">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="64"/>
       <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="51">
+      <c r="C14" s="38">
         <v>60</v>
       </c>
-      <c r="D14" s="65">
+      <c r="D14" s="49">
         <v>7250</v>
       </c>
-      <c r="E14" s="65">
+      <c r="E14" s="49">
         <f t="shared" si="0"/>
         <v>7375.6830537042415</v>
       </c>
-      <c r="F14" s="65">
+      <c r="F14" s="49">
         <f t="shared" si="1"/>
         <v>15796.229988423254</v>
       </c>
-      <c r="G14" s="70">
+      <c r="G14" s="54">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="H14" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="51">
+      <c r="C15" s="38">
         <v>70</v>
       </c>
-      <c r="D15" s="65">
+      <c r="D15" s="49">
         <v>8632</v>
       </c>
-      <c r="E15" s="65">
+      <c r="E15" s="49">
         <f t="shared" si="0"/>
         <v>8246.2579495201171</v>
       </c>
-      <c r="F15" s="65">
+      <c r="F15" s="49">
         <f t="shared" si="1"/>
         <v>148796.92950842451</v>
       </c>
-      <c r="G15" s="70">
+      <c r="G15" s="54">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="51">
+      <c r="C16" s="38">
         <v>72</v>
       </c>
-      <c r="D16" s="65">
+      <c r="D16" s="49">
         <v>6964</v>
       </c>
-      <c r="E16" s="65">
+      <c r="E16" s="49">
         <f t="shared" si="0"/>
         <v>8408.0744505186685</v>
       </c>
-      <c r="F16" s="65">
+      <c r="F16" s="49">
         <f t="shared" si="1"/>
         <v>2085351.0186407943</v>
       </c>
-      <c r="G16" s="70">
+      <c r="G16" s="54">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="51">
+      <c r="C17" s="38">
         <v>90</v>
       </c>
-      <c r="D17" s="65">
+      <c r="D17" s="49">
         <v>11097</v>
       </c>
-      <c r="E17" s="65">
+      <c r="E17" s="49">
         <f t="shared" si="0"/>
         <v>9679.945787036293</v>
       </c>
-      <c r="F17" s="65">
+      <c r="F17" s="49">
         <f t="shared" si="1"/>
         <v>2008042.6424781911</v>
       </c>
-      <c r="G17" s="70">
+      <c r="G17" s="54">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
-      <c r="B18" s="47" t="s">
+      <c r="A18" s="70"/>
+      <c r="B18" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="51">
+      <c r="C18" s="38">
         <v>100</v>
       </c>
-      <c r="D18" s="65">
+      <c r="D18" s="49">
         <v>9107</v>
       </c>
-      <c r="E18" s="65">
+      <c r="E18" s="49">
         <f t="shared" si="0"/>
         <v>10243.058728736596</v>
       </c>
-      <c r="F18" s="65">
+      <c r="F18" s="49">
         <f t="shared" si="1"/>
         <v>1290629.4351386109</v>
       </c>
-      <c r="G18" s="70">
+      <c r="G18" s="54">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="10.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="65"/>
+      <c r="B19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="52">
+      <c r="C19" s="39">
         <v>168</v>
       </c>
-      <c r="D19" s="67">
+      <c r="D19" s="51">
         <v>11498</v>
       </c>
-      <c r="E19" s="67">
+      <c r="E19" s="51">
         <f t="shared" si="0"/>
         <v>11354.263057917007</v>
       </c>
-      <c r="F19" s="67">
+      <c r="F19" s="51">
         <f t="shared" si="1"/>
         <v>20660.308519369613</v>
       </c>
-      <c r="G19" s="71">
+      <c r="G19" s="55">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="H19" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="28">
+      <c r="I19" s="20">
         <v>0</v>
       </c>
     </row>
@@ -2768,15 +2767,64 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <_dlc_DocId xmlns="acade835-edac-4a7e-af34-56d289d23a02">YMK2ZCXUH6A7-1062-164</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="acade835-edac-4a7e-af34-56d289d23a02">
+      <Url>https://eis.usafa.edu/academics/management/or310spring2015/_layouts/DocIdRedir.aspx?ID=YMK2ZCXUH6A7-1062-164</Url>
+      <Description>YMK2ZCXUH6A7-1062-164</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F3F656F81252624C938D713874C0B055" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="700373c59ae5d47123d43a4fe60a5c5f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="acade835-edac-4a7e-af34-56d289d23a02" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e656474fba557ba86c707fc324b95e8" ns2:_="">
     <xsd:import namespace="acade835-edac-4a7e-af34-56d289d23a02"/>
@@ -2921,73 +2969,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <_dlc_DocId xmlns="acade835-edac-4a7e-af34-56d289d23a02">YMK2ZCXUH6A7-1062-164</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="acade835-edac-4a7e-af34-56d289d23a02">
-      <Url>https://eis.usafa.edu/academics/management/or310spring2015/_layouts/DocIdRedir.aspx?ID=YMK2ZCXUH6A7-1062-164</Url>
-      <Description>YMK2ZCXUH6A7-1062-164</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8C6EB0C-451E-4D3D-9E7B-ED62E425E563}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B59F633-A8F9-42AC-9F1F-0B7F8210D11A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="acade835-edac-4a7e-af34-56d289d23a02"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EF6503B-51A4-42DA-8A0B-7604897BCC7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B991A7C-6498-418D-836E-3B3FBC97AB2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3005,26 +3020,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EF6503B-51A4-42DA-8A0B-7604897BCC7E}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8C6EB0C-451E-4D3D-9E7B-ED62E425E563}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B59F633-A8F9-42AC-9F1F-0B7F8210D11A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="acade835-edac-4a7e-af34-56d289d23a02"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>